<commit_message>
Ticker list xlsx updt
</commit_message>
<xml_diff>
--- a/ticker_list.xlsx
+++ b/ticker_list.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>BAJAJ-AUTO.NS</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>IRCTC.NS</t>
-  </si>
-  <si>
-    <t>TATACHEM.NS</t>
   </si>
 </sst>
 </file>
@@ -921,7 +918,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF1"/>
+  <dimension ref="A1:AE1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <selection activeCell="AF2" sqref="AF2"/>
@@ -929,7 +926,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1022,9 +1019,6 @@
       </c>
       <c r="AE1" t="s">
         <v>30</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>